<commit_message>
added code for Excel reading
</commit_message>
<xml_diff>
--- a/MavenFirstProject/src/test/resources/testData/AppData.xlsx
+++ b/MavenFirstProject/src/test/resources/testData/AppData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\JavaWorkspace\MavenFirstProject\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitAutomation\13thJan-2022\MavenFirstProject\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDA75E2-E1B9-40EE-AE64-062AEE298EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E025C8A6-43E1-42DA-9594-D1C1FDEB41C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>AppUrl</t>
   </si>
@@ -65,13 +65,17 @@
   </si>
   <si>
     <t>vtiger</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,15 +399,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -435,6 +439,9 @@
       </c>
       <c r="D2" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>